<commit_message>
logo and title test
</commit_message>
<xml_diff>
--- a/MyFramework1/TestData/Data.xlsx
+++ b/MyFramework1/TestData/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakunthaladilini/Desktop/Eclips/SQAAssignment/MyFramework1/TestData/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sakunthaladilini/git/Framework/MyFramework1/TestData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{105E2425-601B-7544-954F-000BE3E5DB1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96897FD9-28CA-504F-A462-43E46E2A987A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16560" xr2:uid="{41CE2AFC-A77C-BC47-9E6D-233151D4610B}"/>
   </bookViews>
@@ -26,12 +26,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>sakunthalanfm@gmail.com</t>
   </si>
   <si>
-    <t>saku@123</t>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Saku@123</t>
   </si>
 </sst>
 </file>
@@ -76,9 +82,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -394,10 +403,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C82CDCF-78E8-8C41-A208-E098D5EC2FF5}">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -407,17 +416,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
+      <c r="B2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{090DAA8D-3130-7240-90C9-EDB5B314A941}"/>
-    <hyperlink ref="A1" r:id="rId2" xr:uid="{AC8BDC0E-4143-174C-94CE-AF75A645CC0A}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{090DAA8D-3130-7240-90C9-EDB5B314A941}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{AC8BDC0E-4143-174C-94CE-AF75A645CC0A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>